<commit_message>
done changes for create account page test and few other changes
</commit_message>
<xml_diff>
--- a/MyStore/src/main/java/com/testData/userCredentials.xlsx
+++ b/MyStore/src/main/java/com/testData/userCredentials.xlsx
@@ -72,13 +72,13 @@
     <t>California</t>
   </si>
   <si>
-    <t>Nidhi</t>
-  </si>
-  <si>
-    <t>nidhip</t>
-  </si>
-  <si>
-    <t>nidp@gmail.com</t>
+    <t>Sidhi</t>
+  </si>
+  <si>
+    <t>sidhip</t>
+  </si>
+  <si>
+    <t>sidp@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>